<commit_message>
Added : Data set selections
</commit_message>
<xml_diff>
--- a/Deliverables/20221012SpecsOutputs.xlsx
+++ b/Deliverables/20221012SpecsOutputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boiss\Desktop\Cours\PR&amp;D Deep Agora\Deep-Agora_DOC\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C480D146-699A-4F40-BEB3-95CBCD808A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB01A68-2B2C-40F0-B137-537E82497DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="637" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
   <si>
     <t>Description</t>
   </si>
@@ -59,15 +59,6 @@
     <t>legend</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -549,9 +540,6 @@
   </si>
   <si>
     <t>Summary table of the different EOCs that may be searched for</t>
-  </si>
-  <si>
-    <t>Extractors</t>
   </si>
   <si>
     <t>Use cases:</t>
@@ -854,6 +842,38 @@
     </r>
   </si>
   <si>
+    <t>illustration</t>
+  </si>
+  <si>
+    <t>page frames</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">On the sides of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doc</t>
+    </r>
+  </si>
+  <si>
+    <t>Wooden frame on the sides of the page</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -873,11 +893,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 3.0</t>
-    </r>
-  </si>
-  <si>
-    <t>illustration</t>
+      <t xml:space="preserve"> 3.1</t>
+    </r>
+  </si>
+  <si>
+    <t>Handwritten annotation</t>
+  </si>
+  <si>
+    <t>Characters</t>
+  </si>
+  <si>
+    <t>Extractors of</t>
+  </si>
+  <si>
+    <t>Decorations</t>
+  </si>
+  <si>
+    <t>Text-Lines</t>
   </si>
 </sst>
 </file>
@@ -917,14 +949,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1077,7 +1109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1121,86 +1153,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1482,11 +1523,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1496,460 +1535,493 @@
     <col min="4" max="4" width="15.5546875" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" style="11" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="11"/>
+    <col min="7" max="10" width="12.77734375" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="31" t="s">
+      <c r="D6" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="40"/>
+    </row>
+    <row r="9" spans="1:10" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="30"/>
-    </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
-        <v>67</v>
+      <c r="F9" s="38"/>
+      <c r="G9" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>17</v>
+        <v>65</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>14</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
-        <v>15</v>
+      <c r="H10" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="33"/>
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="34"/>
+        <v>20</v>
+      </c>
+      <c r="D11" s="42"/>
       <c r="E11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
-        <v>52</v>
+      <c r="H11" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="33"/>
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="34"/>
+        <v>57</v>
+      </c>
+      <c r="D12" s="42"/>
       <c r="E12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="33"/>
+      <c r="H12" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-    </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
-        <v>51</v>
+      <c r="I12" s="33"/>
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="36" t="s">
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="34"/>
+        <v>21</v>
+      </c>
+      <c r="D13" s="42"/>
       <c r="E13" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="33"/>
+      <c r="H13" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
-        <v>65</v>
+      <c r="I13" s="33"/>
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="34"/>
+        <v>73</v>
+      </c>
+      <c r="D14" s="42"/>
       <c r="E14" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
         <v>49</v>
       </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="32"/>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="B15" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="34"/>
+        <v>74</v>
+      </c>
+      <c r="D15" s="42"/>
       <c r="E15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="G15" s="33"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="32"/>
+    </row>
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="34"/>
+        <v>22</v>
+      </c>
+      <c r="D16" s="42"/>
       <c r="E16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
-        <v>22</v>
+        <v>51</v>
+      </c>
+      <c r="G16" s="33"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="32"/>
+    </row>
+    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="34"/>
+        <v>23</v>
+      </c>
+      <c r="D17" s="42"/>
       <c r="E17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="33"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="32"/>
+    </row>
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="34"/>
+        <v>24</v>
+      </c>
+      <c r="D18" s="42"/>
       <c r="E18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="32"/>
+    </row>
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="43"/>
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="33"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="32"/>
+    </row>
+    <row r="21" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="33"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="32"/>
+    </row>
+    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="15" t="s">
+      <c r="C22" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="42"/>
+      <c r="E22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="33"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="34"/>
+      <c r="J22" s="32"/>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="42"/>
       <c r="E23" s="4" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-    </row>
-    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
-        <v>75</v>
+        <v>60</v>
+      </c>
+      <c r="G23" s="33"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="32"/>
+    </row>
+    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="34"/>
+        <v>24</v>
+      </c>
+      <c r="D24" s="42"/>
       <c r="E24" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E35" s="19"/>
+        <v>52</v>
+      </c>
+      <c r="G24" s="33"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="32"/>
+    </row>
+    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="42"/>
+      <c r="E25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="33"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="32"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D10:D19"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>